<commit_message>
Adicionando BR2019, BR2018 e BR2017
</commit_message>
<xml_diff>
--- a/de_para_siglas_br.xlsx
+++ b/de_para_siglas_br.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\Google Drive\Projetos\SofaScore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0959739-2F8C-4833-8590-E2C36882F580}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA2CE6A-C25E-47B0-B31C-7FC57F8EDE5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{DEF87676-18A4-4917-8F84-01865B9D76F3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DEF87676-18A4-4917-8F84-01865B9D76F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="96">
   <si>
     <t>PAL</t>
   </si>
@@ -313,6 +313,15 @@
   </si>
   <si>
     <t>Paraná</t>
+  </si>
+  <si>
+    <t>CSA</t>
+  </si>
+  <si>
+    <t>Fortaleza</t>
+  </si>
+  <si>
+    <t>FOR</t>
   </si>
 </sst>
 </file>
@@ -667,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7544FCF-6322-4828-A632-33DF8CF41F55}">
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,6 +1120,22 @@
         <v>17</v>
       </c>
     </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B39" xr:uid="{877B5286-E4C9-4175-BFDD-9F327F63BB98}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B39">

</xml_diff>